<commit_message>
Hoàn thành form Quản lý danh sách câu hỏi (và đáp án kèm theo). Thêm bảng CapDo vào database. Insert thêm 11 câu hỏi với 4 cấp độ trong db
</commit_message>
<xml_diff>
--- a/PhieuVanDap - CD2017_1 - v0.1.xlsx
+++ b/PhieuVanDap - CD2017_1 - v0.1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lập trình\Năm 4 - HK1\Lập trình ứng dụng quản lý 1\ĐỒ ÁN QUẢN LÝ THI TRẮC NGHIỆM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lập trình\Năm 4 - HK1\Lập trình ứng dụng quản lý 1\DA-LTUDQL1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B5DB44-5FB0-4E17-B6B3-E00CE22F6CA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE12477-16A9-405D-A90E-C3613C9E76B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Lưu ý:</t>
   </si>
@@ -242,6 +242,18 @@
   </si>
   <si>
     <t>Không sử dụng Data Binding</t>
+  </si>
+  <si>
+    <t>Trần Khôi</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Lý</t>
+  </si>
+  <si>
+    <t>Lê Thanh Bình</t>
+  </si>
+  <si>
+    <t>Phan Xiêu Thiên</t>
   </si>
 </sst>
 </file>
@@ -897,7 +909,7 @@
   <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -924,7 +936,9 @@
       <c r="A2" s="30">
         <v>1</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="31" t="s">
+        <v>69</v>
+      </c>
       <c r="C2" s="32"/>
       <c r="D2" s="33"/>
     </row>
@@ -932,7 +946,9 @@
       <c r="A3" s="34">
         <v>2</v>
       </c>
-      <c r="B3" s="35"/>
+      <c r="B3" s="35" t="s">
+        <v>70</v>
+      </c>
       <c r="C3" s="36"/>
       <c r="D3" s="37"/>
     </row>
@@ -940,7 +956,9 @@
       <c r="A4" s="34">
         <v>3</v>
       </c>
-      <c r="B4" s="35"/>
+      <c r="B4" s="35" t="s">
+        <v>71</v>
+      </c>
       <c r="C4" s="36"/>
       <c r="D4" s="37"/>
     </row>
@@ -948,7 +966,9 @@
       <c r="A5" s="34">
         <v>4</v>
       </c>
-      <c r="B5" s="35"/>
+      <c r="B5" s="35" t="s">
+        <v>72</v>
+      </c>
       <c r="C5" s="36"/>
       <c r="D5" s="37"/>
     </row>

</xml_diff>